<commit_message>
stand für Anhörung abgeben
</commit_message>
<xml_diff>
--- a/LWB_Regionale_Biodiversitaet_Landschaftsqualitaet_V1_0_Kataloge.xlsx
+++ b/LWB_Regionale_Biodiversitaet_Landschaftsqualitaet_V1_0_Kataloge.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_SOURCE\blw-ofag-ufag-Kulturflaechen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\CH BLW 01-00 Interlis und GIS Support\Tasks\BrBL Modelldokumentation\Lieferobjekte\20250508\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D56302-5387-4383-B3B3-5FA13AF43167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F86072F-6E04-46AD-90E5-1749E662F3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{C396946F-947F-4E79-B714-7262D8D2C1C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{C396946F-947F-4E79-B714-7262D8D2C1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Katalog Massnahmen" sheetId="1" r:id="rId1"/>
-    <sheet name="Katalog Foerderkategorien" sheetId="2" r:id="rId2"/>
-    <sheet name="Auswahlliste_Massn_Kategorien" sheetId="3" r:id="rId3"/>
+    <sheet name="Katalog MassnahmenKategorien" sheetId="3" r:id="rId2"/>
+    <sheet name="Katalog Foerderkategorien" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="104">
   <si>
     <t>tid</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Kategorie</t>
   </si>
   <si>
-    <t>Anrechenbar_fuer_OeLN_und_Spezialkulturen</t>
-  </si>
-  <si>
     <t>Gueltig_Bis</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>Ackerflaeche</t>
   </si>
   <si>
-    <t>Ackerbegleitflora (Einsaat oder spontane/autochthone)</t>
-  </si>
-  <si>
     <t>Heckenpflanzung</t>
   </si>
   <si>
@@ -94,9 +88,6 @@
     <t>Pflege einer Nicht-BFF-Hecke</t>
   </si>
   <si>
-    <t>Schwerpunktraum</t>
-  </si>
-  <si>
     <t>Diverses</t>
   </si>
   <si>
@@ -106,24 +97,12 @@
     <t>Feuchtgebiete</t>
   </si>
   <si>
-    <t>Pflege von Tümpeln und Teichen</t>
-  </si>
-  <si>
-    <t>Neuansaat von Wiesen durch Direktbegrünung</t>
-  </si>
-  <si>
     <t>Dauerwiesen</t>
   </si>
   <si>
     <t>Gestaffelte Nutzung auf Betriebsebene</t>
   </si>
   <si>
-    <t>regionale Massnahme Schwerpunkt Biodiversität (z.B. Kiebizfläche)</t>
-  </si>
-  <si>
-    <t>regionale_Massnahme</t>
-  </si>
-  <si>
     <t>Pflanzung von einheimischen Einzelbäumen und Hochstammfeldobstbäumen</t>
   </si>
   <si>
@@ -152,13 +131,232 @@
   </si>
   <si>
     <t>Gueltig_Von</t>
+  </si>
+  <si>
+    <t>Anrechenbar_an_OeLN</t>
+  </si>
+  <si>
+    <t>Zusatzbeitrag in einem Fördergebiet</t>
+  </si>
+  <si>
+    <t>Mit Heugras- oder Heudruschsaaten neuangesäte Wiesen</t>
+  </si>
+  <si>
+    <t>Mit regional angepasstem Saatgut neuangesäte Wiesen</t>
+  </si>
+  <si>
+    <t>Ackerbegleitflora (spontane/autochthone oder Einsaat)</t>
+  </si>
+  <si>
+    <t>Erhaltung und Pflege von Tümpeln und Teichen</t>
+  </si>
+  <si>
+    <t>Cultures principales colorées</t>
+  </si>
+  <si>
+    <t>Flore accompagnatrice des cultures (spontanée/autochthone ou semis)</t>
+  </si>
+  <si>
+    <t>Plantation de haies</t>
+  </si>
+  <si>
+    <t>Entretien de haies non-SPB</t>
+  </si>
+  <si>
+    <t>Contribution supplémentaire dans une zone de promotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en place de mares et d’étangs </t>
+  </si>
+  <si>
+    <t>Maintien et entretien des mares et étangs</t>
+  </si>
+  <si>
+    <t>Prairies nouvellement ensemencées avec des semences de prairie ou de foin</t>
+  </si>
+  <si>
+    <t>Prairies réensemencées avec des semences adaptées à la région</t>
+  </si>
+  <si>
+    <t>Utilisation échelonnée au niveau de l’exploitation</t>
+  </si>
+  <si>
+    <t>Plantation d’arbres isolés indigènes et d’arbres fruitiers haute-tige</t>
+  </si>
+  <si>
+    <t>Entretien d’arbres isolés indigènes</t>
+  </si>
+  <si>
+    <t>Maintien et entretien des murs en pierres sèches</t>
+  </si>
+  <si>
+    <t>Création, maintien et entretien des petites structures</t>
+  </si>
+  <si>
+    <t>Colture principali colorate</t>
+  </si>
+  <si>
+    <t>Flora segetale (spontanea/autoctona o seminata)</t>
+  </si>
+  <si>
+    <t>Piantagione di siepi</t>
+  </si>
+  <si>
+    <t>Cura di siepi che non sono di tipo SPB</t>
+  </si>
+  <si>
+    <t>Contributo supplementare in una zona di promozione</t>
+  </si>
+  <si>
+    <t>Creazione, mantenimento e cura di piccole strutture</t>
+  </si>
+  <si>
+    <t>Piantagione di alberi indigeni isolati e di alberi da frutto ad alto fusto nei campi</t>
+  </si>
+  <si>
+    <t>Cura di alberi indigeni isolati</t>
+  </si>
+  <si>
+    <t>Predisposizione di stagni e pozze</t>
+  </si>
+  <si>
+    <t>Mantenimento e cura di stagni e pozze</t>
+  </si>
+  <si>
+    <t>Mantenimento e cura di muri a secco</t>
+  </si>
+  <si>
+    <t>Prati riseminati con fiorume o semente prativa</t>
+  </si>
+  <si>
+    <t>Prati riseminati con sementi adeguate alla regione</t>
+  </si>
+  <si>
+    <t>Utilizzo scaglionato a livello di azienda</t>
+  </si>
+  <si>
+    <t>Anwendung_Kt</t>
+  </si>
+  <si>
+    <t>Regionale_Massnahme</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.m14</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.m1</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.m2</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.m3</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.m4</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.m5</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.m6</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.m7</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.m8</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.m9</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.m10</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.m11</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.m12</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.m13</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.mk1</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.mk2</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.mk3</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.mk4</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.mk5</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.mk6</t>
+  </si>
+  <si>
+    <t>ch.admin.blw.elemente_regionale_biodiversitaet_landschaftsqualitaet.fk0</t>
+  </si>
+  <si>
+    <t>Beispieleintrag!</t>
+  </si>
+  <si>
+    <t>Terres assolées</t>
+  </si>
+  <si>
+    <t>Superficie coltiva</t>
+  </si>
+  <si>
+    <t>Haies et arbres</t>
+  </si>
+  <si>
+    <t>Divers</t>
+  </si>
+  <si>
+    <t>Altro</t>
+  </si>
+  <si>
+    <t>Zones humides</t>
+  </si>
+  <si>
+    <t>Aree umide</t>
+  </si>
+  <si>
+    <t>Prairies permanentes</t>
+  </si>
+  <si>
+    <t>Prati perenni</t>
+  </si>
+  <si>
+    <t>Structures</t>
+  </si>
+  <si>
+    <t>Strutture</t>
+  </si>
+  <si>
+    <t>Hecken und Baeume</t>
+  </si>
+  <si>
+    <t>Siepi e alberi</t>
+  </si>
+  <si>
+    <t>Alouette des champs</t>
+  </si>
+  <si>
+    <t>Allodola</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +376,25 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -203,10 +420,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -541,27 +760,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9795B9D3-1595-41AA-844B-8EBE47E903E3}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.7109375" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="70.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="10" width="23.7109375" customWidth="1"/>
+    <col min="11" max="11" width="26.140625" customWidth="1"/>
+    <col min="12" max="13" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,338 +804,667 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>72</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="J6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>74</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>75</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>62</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>76</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
         <v>25</v>
       </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
+      <c r="J12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>57</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="J13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>80</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
         <v>14</v>
+      </c>
+      <c r="J14" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>67</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>61</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="I15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E077B6-4C45-48E0-9377-4C4473DEE1B8}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A9322ED-9E79-4A43-90B9-174A2F8835E7}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -924,117 +1473,245 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A9322ED-9E79-4A43-90B9-174A2F8835E7}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Versionsdatum xmlns="558044cc-f176-4c91-a0e4-bc704674ebff" xsi:nil="true"/>
+    <Dokument_x0020_Status xmlns="558044cc-f176-4c91-a0e4-bc704674ebff">Vorlage</Dokument_x0020_Status>
+    <Dokument_x0020_Version xmlns="558044cc-f176-4c91-a0e4-bc704674ebff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E077B6-4C45-48E0-9377-4C4473DEE1B8}">
-  <dimension ref="A1:A8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Arbeitsdokumente" ma:contentTypeID="0x0101002F9FFC2F4692C040A9D99914B314900F00A01FF6A596BD62458797012A75898D40" ma:contentTypeVersion="" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="2dc8e0ecbea582e163f01a1b80039e01">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="558044cc-f176-4c91-a0e4-bc704674ebff" xmlns:ns3="f49360a4-cac7-4495-b78e-580cf2234649" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a392e290f20c9c881d63006c38c23561" ns2:_="" ns3:_="">
+    <xsd:import namespace="558044cc-f176-4c91-a0e4-bc704674ebff"/>
+    <xsd:import namespace="f49360a4-cac7-4495-b78e-580cf2234649"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:Dokument_x0020_Version" minOccurs="0"/>
+                <xsd:element ref="ns2:Versionsdatum" minOccurs="0"/>
+                <xsd:element ref="ns2:Dokument_x0020_Status" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="558044cc-f176-4c91-a0e4-bc704674ebff" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Dokument_x0020_Version" ma:index="8" nillable="true" ma:displayName="Dokument Version" ma:description="Im Dokument angezeigte Version. IMMER MANUELL SETZEN!" ma:internalName="Dokument_x0020_Version">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Versionsdatum" ma:index="9" nillable="true" ma:displayName="Versionsdatum" ma:description="Im Dokument angezeigtes Versionsdatum. IMMER MANUELL SETZEN!" ma:internalName="Versionsdatum">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Dokument_x0020_Status" ma:index="10" nillable="true" ma:displayName="Dokument Status" ma:default="Vorlage" ma:format="Dropdown" ma:internalName="Dokument_x0020_Status">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Vorlage"/>
+          <xsd:enumeration value="In Arbeit"/>
+          <xsd:enumeration value="In Prüfung"/>
+          <xsd:enumeration value="Genehmigt zur Nutzung"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f49360a4-cac7-4495-b78e-580cf2234649" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="11" nillable="true" ma:displayName="Freigegeben für" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="12" nillable="true" ma:displayName="Freigegeben für - Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhaltstyp"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA5AE013-4375-4392-8248-516FAC1796A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f49360a4-cac7-4495-b78e-580cf2234649"/>
+    <ds:schemaRef ds:uri="558044cc-f176-4c91-a0e4-bc704674ebff"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{117BCC82-079A-45E3-B6BA-831982416736}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEEDF2B-4216-4962-A7D9-5DF5370993E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="558044cc-f176-4c91-a0e4-bc704674ebff"/>
+    <ds:schemaRef ds:uri="f49360a4-cac7-4495-b78e-580cf2234649"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
finalize fileset after FIG Anhörung
</commit_message>
<xml_diff>
--- a/LWB_Regionale_Biodiversitaet_Landschaftsqualitaet_V1_0_Kataloge.xlsx
+++ b/LWB_Regionale_Biodiversitaet_Landschaftsqualitaet_V1_0_Kataloge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\CH BLW 01-00 Interlis und GIS Support\Tasks\BrBL Modelldokumentation\Lieferobjekte\20250508\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_SOURCE\blw-ofag-ufag-Kulturflaechen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F86072F-6E04-46AD-90E5-1749E662F3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7661F35C-ADCF-43C3-A1F4-0A3129CD48A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{C396946F-947F-4E79-B714-7262D8D2C1C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C396946F-947F-4E79-B714-7262D8D2C1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Katalog Massnahmen" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="104">
   <si>
     <t>tid</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Feuchtgebiete</t>
   </si>
   <si>
-    <t>Dauerwiesen</t>
-  </si>
-  <si>
     <t>Gestaffelte Nutzung auf Betriebsebene</t>
   </si>
   <si>
@@ -133,12 +130,6 @@
     <t>Gueltig_Von</t>
   </si>
   <si>
-    <t>Anrechenbar_an_OeLN</t>
-  </si>
-  <si>
-    <t>Zusatzbeitrag in einem Fördergebiet</t>
-  </si>
-  <si>
     <t>Mit Heugras- oder Heudruschsaaten neuangesäte Wiesen</t>
   </si>
   <si>
@@ -163,9 +154,6 @@
     <t>Entretien de haies non-SPB</t>
   </si>
   <si>
-    <t>Contribution supplémentaire dans une zone de promotion</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mise en place de mares et d’étangs </t>
   </si>
   <si>
@@ -205,9 +193,6 @@
     <t>Cura di siepi che non sono di tipo SPB</t>
   </si>
   <si>
-    <t>Contributo supplementare in una zona di promozione</t>
-  </si>
-  <si>
     <t>Creazione, mantenimento e cura di piccole strutture</t>
   </si>
   <si>
@@ -328,21 +313,12 @@
     <t>Aree umide</t>
   </si>
   <si>
-    <t>Prairies permanentes</t>
-  </si>
-  <si>
-    <t>Prati perenni</t>
-  </si>
-  <si>
     <t>Structures</t>
   </si>
   <si>
     <t>Strutture</t>
   </si>
   <si>
-    <t>Hecken und Baeume</t>
-  </si>
-  <si>
     <t>Siepi e alberi</t>
   </si>
   <si>
@@ -350,6 +326,30 @@
   </si>
   <si>
     <t>Allodola</t>
+  </si>
+  <si>
+    <t>Dauergrünflächen</t>
+  </si>
+  <si>
+    <t>Surfaces herbagères permanentes</t>
+  </si>
+  <si>
+    <t>Superficie permanentemente inerbita</t>
+  </si>
+  <si>
+    <t>Hecken und Bäume</t>
+  </si>
+  <si>
+    <t>Ackerfläche</t>
+  </si>
+  <si>
+    <t>Gebietsspezifischer Zusatzbeitrag</t>
+  </si>
+  <si>
+    <t>contribution supplémentaire spécifique à la zone</t>
+  </si>
+  <si>
+    <t>Contributo supplementare specifico del comprensorio</t>
   </si>
 </sst>
 </file>
@@ -760,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9795B9D3-1595-41AA-844B-8EBE47E903E3}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,12 +776,12 @@
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="10" width="23.7109375" customWidth="1"/>
-    <col min="11" max="11" width="26.140625" customWidth="1"/>
-    <col min="12" max="13" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" customWidth="1"/>
+    <col min="11" max="12" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -804,27 +804,24 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -833,10 +830,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -850,25 +847,22 @@
       <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -882,13 +876,10 @@
       <c r="J3" t="s">
         <v>11</v>
       </c>
-      <c r="K3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -897,10 +888,10 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -912,15 +903,12 @@
         <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -929,10 +917,10 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -946,25 +934,22 @@
       <c r="J5" t="s">
         <v>11</v>
       </c>
-      <c r="K5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -978,13 +963,10 @@
       <c r="J6" t="s">
         <v>11</v>
       </c>
-      <c r="K6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -993,10 +975,10 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -1008,27 +990,24 @@
         <v>18</v>
       </c>
       <c r="J7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -1040,27 +1019,24 @@
         <v>18</v>
       </c>
       <c r="J8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
@@ -1069,30 +1045,27 @@
         <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="J9" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
@@ -1101,94 +1074,85 @@
         <v>10</v>
       </c>
       <c r="I10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="J10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
       <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
         <v>46</v>
       </c>
-      <c r="E11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
         <v>24</v>
       </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" t="s">
-        <v>25</v>
-      </c>
       <c r="J12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
         <v>10</v>
@@ -1200,27 +1164,24 @@
         <v>14</v>
       </c>
       <c r="J13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
@@ -1232,27 +1193,24 @@
         <v>14</v>
       </c>
       <c r="J14" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
         <v>10</v>
@@ -1264,9 +1222,6 @@
         <v>16</v>
       </c>
       <c r="J15" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1282,15 +1237,15 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1298,16 +1253,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
@@ -1315,91 +1270,92 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" t="s">
         <v>97</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>99</v>
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1407,7 +1363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A9322ED-9E79-4A43-90B9-174A2F8835E7}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -1428,19 +1384,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>8</v>
@@ -1449,22 +1405,22 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>